<commit_message>
Align sector and document names in transport with the rest of the model
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_TRA_EV_Parity.xlsx
+++ b/SuppXLS/Scen_B_TRA_EV_Parity.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\TIM\SuppXLS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2435B31B-D2E5-46FB-933C-A3D49910FBDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CE92432-3F97-43C3-8590-680A1E96AFDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="12852" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="17" r:id="rId1"/>
@@ -1047,16 +1047,16 @@
     <t>https://creativecommons.org/licenses/by-nc-sa/4.0/</t>
   </si>
   <si>
-    <t>Scenario file</t>
-  </si>
-  <si>
-    <t>Transport (TRA)</t>
-  </si>
-  <si>
     <t>Vahid Aryanpur (UCC, vahid.aryanpur@ucc.ie)</t>
   </si>
   <si>
     <t>Purchase price parity for EVs</t>
+  </si>
+  <si>
+    <t>Scenario</t>
+  </si>
+  <si>
+    <t>Transport sector (TRA)</t>
   </si>
 </sst>
 </file>
@@ -1606,7 +1606,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1D6391F9-D113-4D54-B2C5-E7E4BCEE0804}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1650,7 +1650,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7C68D2FA-16D1-4C4A-A1B4-F5EF71E3ABEA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1699,7 +1699,7 @@
         <xdr:cNvPr id="4" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B58D1E47-C0BF-43AD-86E7-9DB305BD8904}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1749,7 +1749,7 @@
         <xdr:cNvPr id="5" name="Picture 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DE167750-D03F-47FD-8C68-42FE8DC6BDDC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1799,7 +1799,7 @@
         <xdr:cNvPr id="6" name="Picture 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D80462FA-3219-4DA6-B3FE-360C76C31D93}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1848,7 +1848,7 @@
         <xdr:cNvPr id="7" name="Picture 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D0694059-E3D4-4271-8205-842727E8A2DB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
             </a:ext>
             <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
               <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{B1489C0F-1609-4587-A5BA-D0B99739EA08}"/>
@@ -1908,7 +1908,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>22860</xdr:colOff>
+          <xdr:colOff>19050</xdr:colOff>
           <xdr:row>3</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
@@ -2283,24 +2283,24 @@
   <dimension ref="A1:Z99"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20:D20"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" width="21.6640625" style="14" customWidth="1"/>
-    <col min="5" max="6" width="14.109375" style="14" customWidth="1"/>
-    <col min="7" max="7" width="12.109375" style="14" customWidth="1"/>
-    <col min="8" max="10" width="8.109375" style="14" customWidth="1"/>
-    <col min="11" max="11" width="9.6640625" style="14" customWidth="1"/>
-    <col min="12" max="12" width="8.109375" style="14" customWidth="1"/>
+    <col min="1" max="4" width="21.7109375" style="14" customWidth="1"/>
+    <col min="5" max="6" width="14.140625" style="14" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" style="14" customWidth="1"/>
+    <col min="8" max="10" width="8.140625" style="14" customWidth="1"/>
+    <col min="11" max="11" width="9.7109375" style="14" customWidth="1"/>
+    <col min="12" max="12" width="8.140625" style="14" customWidth="1"/>
     <col min="13" max="13" width="10" style="14" customWidth="1"/>
-    <col min="14" max="14" width="11.44140625" style="14" customWidth="1"/>
-    <col min="15" max="15" width="13.44140625" style="14" customWidth="1"/>
-    <col min="16" max="16384" width="8.88671875" style="14"/>
+    <col min="14" max="14" width="11.42578125" style="14" customWidth="1"/>
+    <col min="15" max="15" width="13.42578125" style="14" customWidth="1"/>
+    <col min="16" max="16384" width="8.85546875" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" s="50"/>
       <c r="B1" s="50"/>
       <c r="C1" s="50"/>
@@ -2328,7 +2328,7 @@
       <c r="Y1" s="51"/>
       <c r="Z1" s="51"/>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" s="50"/>
       <c r="B2" s="50"/>
       <c r="C2" s="50"/>
@@ -2356,7 +2356,7 @@
       <c r="Y2" s="51"/>
       <c r="Z2" s="51"/>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" s="50"/>
       <c r="B3" s="50"/>
       <c r="C3" s="50"/>
@@ -2384,7 +2384,7 @@
       <c r="Y3" s="51"/>
       <c r="Z3" s="51"/>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" s="50"/>
       <c r="B4" s="50"/>
       <c r="C4" s="50"/>
@@ -2412,7 +2412,7 @@
       <c r="Y4" s="51"/>
       <c r="Z4" s="51"/>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" s="50"/>
       <c r="B5" s="50"/>
       <c r="C5" s="50"/>
@@ -2440,7 +2440,7 @@
       <c r="Y5" s="51"/>
       <c r="Z5" s="51"/>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" s="50"/>
       <c r="B6" s="50"/>
       <c r="C6" s="50"/>
@@ -2468,7 +2468,7 @@
       <c r="Y6" s="51"/>
       <c r="Z6" s="51"/>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" s="50"/>
       <c r="B7" s="50"/>
       <c r="C7" s="50"/>
@@ -2496,7 +2496,7 @@
       <c r="Y7" s="51"/>
       <c r="Z7" s="51"/>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" s="50"/>
       <c r="B8" s="50"/>
       <c r="C8" s="50"/>
@@ -2524,7 +2524,7 @@
       <c r="Y8" s="51"/>
       <c r="Z8" s="51"/>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" s="50"/>
       <c r="B9" s="50"/>
       <c r="C9" s="50"/>
@@ -2552,7 +2552,7 @@
       <c r="Y9" s="51"/>
       <c r="Z9" s="51"/>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" s="50"/>
       <c r="B10" s="50"/>
       <c r="C10" s="50"/>
@@ -2580,7 +2580,7 @@
       <c r="Y10" s="51"/>
       <c r="Z10" s="51"/>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" s="50"/>
       <c r="B11" s="50"/>
       <c r="C11" s="50"/>
@@ -2608,7 +2608,7 @@
       <c r="Y11" s="51"/>
       <c r="Z11" s="51"/>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" s="50"/>
       <c r="B12" s="50"/>
       <c r="C12" s="50"/>
@@ -2636,7 +2636,7 @@
       <c r="Y12" s="51"/>
       <c r="Z12" s="51"/>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A13" s="50"/>
       <c r="B13" s="50"/>
       <c r="C13" s="50"/>
@@ -2664,7 +2664,7 @@
       <c r="Y13" s="51"/>
       <c r="Z13" s="51"/>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A14" s="50"/>
       <c r="B14" s="50"/>
       <c r="C14" s="50"/>
@@ -2692,7 +2692,7 @@
       <c r="Y14" s="51"/>
       <c r="Z14" s="51"/>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A15" s="50"/>
       <c r="B15" s="50"/>
       <c r="C15" s="50"/>
@@ -2720,7 +2720,7 @@
       <c r="Y15" s="51"/>
       <c r="Z15" s="51"/>
     </row>
-    <row r="16" spans="1:26" ht="102.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:26" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="66" t="s">
         <v>232</v>
       </c>
@@ -2750,7 +2750,7 @@
       <c r="Y16" s="51"/>
       <c r="Z16" s="51"/>
     </row>
-    <row r="17" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="54"/>
       <c r="B17" s="54"/>
       <c r="C17" s="54"/>
@@ -2778,7 +2778,7 @@
       <c r="Y17" s="51"/>
       <c r="Z17" s="51"/>
     </row>
-    <row r="18" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="54"/>
       <c r="B18" s="54"/>
       <c r="C18" s="54"/>
@@ -2806,12 +2806,12 @@
       <c r="Y18" s="51"/>
       <c r="Z18" s="51"/>
     </row>
-    <row r="19" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="57" t="s">
         <v>233</v>
       </c>
       <c r="B19" s="65" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="C19" s="65"/>
       <c r="D19" s="65"/>
@@ -2838,12 +2838,12 @@
       <c r="Y19" s="51"/>
       <c r="Z19" s="51"/>
     </row>
-    <row r="20" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="57" t="s">
         <v>234</v>
       </c>
       <c r="B20" s="65" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="C20" s="65"/>
       <c r="D20" s="65"/>
@@ -2870,12 +2870,12 @@
       <c r="Y20" s="51"/>
       <c r="Z20" s="51"/>
     </row>
-    <row r="21" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="57" t="s">
         <v>235</v>
       </c>
       <c r="B21" s="60" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="C21" s="60"/>
       <c r="D21" s="60"/>
@@ -2902,7 +2902,7 @@
       <c r="Y21" s="51"/>
       <c r="Z21" s="51"/>
     </row>
-    <row r="22" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="57"/>
       <c r="B22" s="60"/>
       <c r="C22" s="60"/>
@@ -2930,12 +2930,12 @@
       <c r="Y22" s="51"/>
       <c r="Z22" s="51"/>
     </row>
-    <row r="23" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="57" t="s">
         <v>236</v>
       </c>
       <c r="B23" s="65" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C23" s="65"/>
       <c r="D23" s="65"/>
@@ -2962,7 +2962,7 @@
       <c r="Y23" s="51"/>
       <c r="Z23" s="51"/>
     </row>
-    <row r="24" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="57"/>
       <c r="B24" s="65"/>
       <c r="C24" s="65"/>
@@ -2990,7 +2990,7 @@
       <c r="Y24" s="51"/>
       <c r="Z24" s="51"/>
     </row>
-    <row r="25" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="57"/>
       <c r="B25" s="60"/>
       <c r="C25" s="60"/>
@@ -3018,12 +3018,12 @@
       <c r="Y25" s="51"/>
       <c r="Z25" s="51"/>
     </row>
-    <row r="26" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="57" t="s">
         <v>237</v>
       </c>
       <c r="B26" s="65" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C26" s="65"/>
       <c r="D26" s="65"/>
@@ -3050,7 +3050,7 @@
       <c r="Y26" s="51"/>
       <c r="Z26" s="51"/>
     </row>
-    <row r="27" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="57"/>
       <c r="B27" s="65"/>
       <c r="C27" s="65"/>
@@ -3078,7 +3078,7 @@
       <c r="Y27" s="51"/>
       <c r="Z27" s="51"/>
     </row>
-    <row r="28" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="57"/>
       <c r="B28" s="60"/>
       <c r="C28" s="60"/>
@@ -3106,7 +3106,7 @@
       <c r="Y28" s="51"/>
       <c r="Z28" s="51"/>
     </row>
-    <row r="29" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="57" t="s">
         <v>238</v>
       </c>
@@ -3138,7 +3138,7 @@
       <c r="Y29" s="51"/>
       <c r="Z29" s="51"/>
     </row>
-    <row r="30" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="57" t="s">
         <v>239</v>
       </c>
@@ -3170,7 +3170,7 @@
       <c r="Y30" s="51"/>
       <c r="Z30" s="51"/>
     </row>
-    <row r="31" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="57" t="s">
         <v>241</v>
       </c>
@@ -3202,7 +3202,7 @@
       <c r="Y31" s="51"/>
       <c r="Z31" s="51"/>
     </row>
-    <row r="32" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="63"/>
       <c r="B32" s="64" t="s">
         <v>243</v>
@@ -3232,7 +3232,7 @@
       <c r="Y32" s="51"/>
       <c r="Z32" s="51"/>
     </row>
-    <row r="33" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A33" s="50"/>
       <c r="B33" s="50"/>
       <c r="C33" s="50"/>
@@ -3260,7 +3260,7 @@
       <c r="Y33" s="51"/>
       <c r="Z33" s="51"/>
     </row>
-    <row r="34" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A34" s="50"/>
       <c r="B34" s="50"/>
       <c r="C34" s="50"/>
@@ -3288,7 +3288,7 @@
       <c r="Y34" s="51"/>
       <c r="Z34" s="51"/>
     </row>
-    <row r="35" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A35" s="50"/>
       <c r="B35" s="50"/>
       <c r="C35" s="50"/>
@@ -3316,7 +3316,7 @@
       <c r="Y35" s="51"/>
       <c r="Z35" s="51"/>
     </row>
-    <row r="36" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A36" s="50"/>
       <c r="B36" s="50"/>
       <c r="C36" s="50"/>
@@ -3344,7 +3344,7 @@
       <c r="Y36" s="51"/>
       <c r="Z36" s="51"/>
     </row>
-    <row r="37" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A37" s="50"/>
       <c r="B37" s="50"/>
       <c r="C37" s="50"/>
@@ -3372,7 +3372,7 @@
       <c r="Y37" s="51"/>
       <c r="Z37" s="51"/>
     </row>
-    <row r="38" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A38" s="50"/>
       <c r="B38" s="50"/>
       <c r="C38" s="50"/>
@@ -3400,7 +3400,7 @@
       <c r="Y38" s="51"/>
       <c r="Z38" s="51"/>
     </row>
-    <row r="39" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A39" s="50"/>
       <c r="B39" s="50"/>
       <c r="C39" s="50"/>
@@ -3428,7 +3428,7 @@
       <c r="Y39" s="51"/>
       <c r="Z39" s="51"/>
     </row>
-    <row r="40" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A40" s="50"/>
       <c r="B40" s="50"/>
       <c r="C40" s="50"/>
@@ -3456,7 +3456,7 @@
       <c r="Y40" s="51"/>
       <c r="Z40" s="51"/>
     </row>
-    <row r="41" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A41" s="50"/>
       <c r="B41" s="50"/>
       <c r="C41" s="50"/>
@@ -3484,7 +3484,7 @@
       <c r="Y41" s="51"/>
       <c r="Z41" s="51"/>
     </row>
-    <row r="42" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A42" s="50"/>
       <c r="B42" s="50"/>
       <c r="C42" s="50"/>
@@ -3512,7 +3512,7 @@
       <c r="Y42" s="51"/>
       <c r="Z42" s="51"/>
     </row>
-    <row r="43" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A43" s="51"/>
       <c r="B43" s="51"/>
       <c r="C43" s="51"/>
@@ -3540,7 +3540,7 @@
       <c r="Y43" s="51"/>
       <c r="Z43" s="51"/>
     </row>
-    <row r="44" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A44" s="51"/>
       <c r="B44" s="51"/>
       <c r="C44" s="51"/>
@@ -3568,7 +3568,7 @@
       <c r="Y44" s="51"/>
       <c r="Z44" s="51"/>
     </row>
-    <row r="45" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A45" s="51"/>
       <c r="B45" s="51"/>
       <c r="C45" s="51"/>
@@ -3596,7 +3596,7 @@
       <c r="Y45" s="51"/>
       <c r="Z45" s="51"/>
     </row>
-    <row r="46" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A46" s="51"/>
       <c r="B46" s="51"/>
       <c r="C46" s="51"/>
@@ -3624,7 +3624,7 @@
       <c r="Y46" s="51"/>
       <c r="Z46" s="51"/>
     </row>
-    <row r="47" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A47" s="51"/>
       <c r="B47" s="51"/>
       <c r="C47" s="51"/>
@@ -3652,7 +3652,7 @@
       <c r="Y47" s="51"/>
       <c r="Z47" s="51"/>
     </row>
-    <row r="48" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A48" s="51"/>
       <c r="B48" s="51"/>
       <c r="C48" s="51"/>
@@ -3680,7 +3680,7 @@
       <c r="Y48" s="51"/>
       <c r="Z48" s="51"/>
     </row>
-    <row r="49" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A49" s="51"/>
       <c r="B49" s="51"/>
       <c r="C49" s="51"/>
@@ -3708,7 +3708,7 @@
       <c r="Y49" s="51"/>
       <c r="Z49" s="51"/>
     </row>
-    <row r="50" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A50" s="51"/>
       <c r="B50" s="51"/>
       <c r="C50" s="51"/>
@@ -3736,7 +3736,7 @@
       <c r="Y50" s="51"/>
       <c r="Z50" s="51"/>
     </row>
-    <row r="51" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A51" s="51"/>
       <c r="B51" s="51"/>
       <c r="C51" s="51"/>
@@ -3764,7 +3764,7 @@
       <c r="Y51" s="51"/>
       <c r="Z51" s="51"/>
     </row>
-    <row r="52" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A52" s="51"/>
       <c r="B52" s="51"/>
       <c r="C52" s="51"/>
@@ -3792,7 +3792,7 @@
       <c r="Y52" s="51"/>
       <c r="Z52" s="51"/>
     </row>
-    <row r="53" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A53" s="51"/>
       <c r="B53" s="51"/>
       <c r="C53" s="51"/>
@@ -3820,7 +3820,7 @@
       <c r="Y53" s="51"/>
       <c r="Z53" s="51"/>
     </row>
-    <row r="54" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A54" s="51"/>
       <c r="B54" s="51"/>
       <c r="C54" s="51"/>
@@ -3848,7 +3848,7 @@
       <c r="Y54" s="51"/>
       <c r="Z54" s="51"/>
     </row>
-    <row r="55" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A55" s="51"/>
       <c r="B55" s="51"/>
       <c r="C55" s="51"/>
@@ -3876,7 +3876,7 @@
       <c r="Y55" s="51"/>
       <c r="Z55" s="51"/>
     </row>
-    <row r="56" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A56" s="51"/>
       <c r="B56" s="51"/>
       <c r="C56" s="51"/>
@@ -3904,7 +3904,7 @@
       <c r="Y56" s="51"/>
       <c r="Z56" s="51"/>
     </row>
-    <row r="57" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A57" s="51"/>
       <c r="B57" s="51"/>
       <c r="C57" s="51"/>
@@ -3932,7 +3932,7 @@
       <c r="Y57" s="51"/>
       <c r="Z57" s="51"/>
     </row>
-    <row r="58" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A58" s="51"/>
       <c r="B58" s="51"/>
       <c r="C58" s="51"/>
@@ -3960,7 +3960,7 @@
       <c r="Y58" s="51"/>
       <c r="Z58" s="51"/>
     </row>
-    <row r="59" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A59" s="51"/>
       <c r="B59" s="51"/>
       <c r="C59" s="51"/>
@@ -3988,7 +3988,7 @@
       <c r="Y59" s="51"/>
       <c r="Z59" s="51"/>
     </row>
-    <row r="60" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A60" s="51"/>
       <c r="B60" s="51"/>
       <c r="C60" s="51"/>
@@ -4016,7 +4016,7 @@
       <c r="Y60" s="51"/>
       <c r="Z60" s="51"/>
     </row>
-    <row r="61" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A61" s="51"/>
       <c r="B61" s="51"/>
       <c r="C61" s="51"/>
@@ -4044,7 +4044,7 @@
       <c r="Y61" s="51"/>
       <c r="Z61" s="51"/>
     </row>
-    <row r="62" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A62" s="51"/>
       <c r="B62" s="51"/>
       <c r="C62" s="51"/>
@@ -4072,7 +4072,7 @@
       <c r="Y62" s="51"/>
       <c r="Z62" s="51"/>
     </row>
-    <row r="63" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A63" s="51"/>
       <c r="B63" s="51"/>
       <c r="C63" s="51"/>
@@ -4100,7 +4100,7 @@
       <c r="Y63" s="51"/>
       <c r="Z63" s="51"/>
     </row>
-    <row r="64" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A64" s="51"/>
       <c r="B64" s="51"/>
       <c r="C64" s="51"/>
@@ -4128,7 +4128,7 @@
       <c r="Y64" s="51"/>
       <c r="Z64" s="51"/>
     </row>
-    <row r="65" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A65" s="51"/>
       <c r="B65" s="51"/>
       <c r="C65" s="51"/>
@@ -4156,7 +4156,7 @@
       <c r="Y65" s="51"/>
       <c r="Z65" s="51"/>
     </row>
-    <row r="66" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A66" s="51"/>
       <c r="B66" s="51"/>
       <c r="C66" s="51"/>
@@ -4184,7 +4184,7 @@
       <c r="Y66" s="51"/>
       <c r="Z66" s="51"/>
     </row>
-    <row r="67" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A67" s="51"/>
       <c r="B67" s="51"/>
       <c r="C67" s="51"/>
@@ -4212,7 +4212,7 @@
       <c r="Y67" s="51"/>
       <c r="Z67" s="51"/>
     </row>
-    <row r="68" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A68" s="51"/>
       <c r="B68" s="51"/>
       <c r="C68" s="51"/>
@@ -4240,7 +4240,7 @@
       <c r="Y68" s="51"/>
       <c r="Z68" s="51"/>
     </row>
-    <row r="69" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A69" s="51"/>
       <c r="B69" s="51"/>
       <c r="C69" s="51"/>
@@ -4268,7 +4268,7 @@
       <c r="Y69" s="51"/>
       <c r="Z69" s="51"/>
     </row>
-    <row r="70" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A70" s="51"/>
       <c r="B70" s="51"/>
       <c r="C70" s="51"/>
@@ -4296,7 +4296,7 @@
       <c r="Y70" s="51"/>
       <c r="Z70" s="51"/>
     </row>
-    <row r="71" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A71" s="51"/>
       <c r="B71" s="51"/>
       <c r="C71" s="51"/>
@@ -4324,7 +4324,7 @@
       <c r="Y71" s="51"/>
       <c r="Z71" s="51"/>
     </row>
-    <row r="72" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A72" s="51"/>
       <c r="B72" s="51"/>
       <c r="C72" s="51"/>
@@ -4352,7 +4352,7 @@
       <c r="Y72" s="51"/>
       <c r="Z72" s="51"/>
     </row>
-    <row r="73" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A73" s="51"/>
       <c r="B73" s="51"/>
       <c r="C73" s="51"/>
@@ -4380,7 +4380,7 @@
       <c r="Y73" s="51"/>
       <c r="Z73" s="51"/>
     </row>
-    <row r="74" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A74" s="51"/>
       <c r="B74" s="51"/>
       <c r="C74" s="51"/>
@@ -4408,7 +4408,7 @@
       <c r="Y74" s="51"/>
       <c r="Z74" s="51"/>
     </row>
-    <row r="75" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A75" s="51"/>
       <c r="B75" s="51"/>
       <c r="C75" s="51"/>
@@ -4436,7 +4436,7 @@
       <c r="Y75" s="51"/>
       <c r="Z75" s="51"/>
     </row>
-    <row r="76" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A76" s="51"/>
       <c r="B76" s="51"/>
       <c r="C76" s="51"/>
@@ -4464,7 +4464,7 @@
       <c r="Y76" s="51"/>
       <c r="Z76" s="51"/>
     </row>
-    <row r="77" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A77" s="51"/>
       <c r="B77" s="51"/>
       <c r="C77" s="51"/>
@@ -4492,7 +4492,7 @@
       <c r="Y77" s="51"/>
       <c r="Z77" s="51"/>
     </row>
-    <row r="78" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A78" s="51"/>
       <c r="B78" s="51"/>
       <c r="C78" s="51"/>
@@ -4520,7 +4520,7 @@
       <c r="Y78" s="51"/>
       <c r="Z78" s="51"/>
     </row>
-    <row r="79" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A79" s="51"/>
       <c r="B79" s="51"/>
       <c r="C79" s="51"/>
@@ -4548,7 +4548,7 @@
       <c r="Y79" s="51"/>
       <c r="Z79" s="51"/>
     </row>
-    <row r="80" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A80" s="51"/>
       <c r="B80" s="51"/>
       <c r="C80" s="51"/>
@@ -4576,7 +4576,7 @@
       <c r="Y80" s="51"/>
       <c r="Z80" s="51"/>
     </row>
-    <row r="81" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A81" s="51"/>
       <c r="B81" s="51"/>
       <c r="C81" s="51"/>
@@ -4604,7 +4604,7 @@
       <c r="Y81" s="51"/>
       <c r="Z81" s="51"/>
     </row>
-    <row r="82" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A82" s="51"/>
       <c r="B82" s="51"/>
       <c r="C82" s="51"/>
@@ -4632,7 +4632,7 @@
       <c r="Y82" s="51"/>
       <c r="Z82" s="51"/>
     </row>
-    <row r="83" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A83" s="51"/>
       <c r="B83" s="51"/>
       <c r="C83" s="51"/>
@@ -4660,7 +4660,7 @@
       <c r="Y83" s="51"/>
       <c r="Z83" s="51"/>
     </row>
-    <row r="84" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A84" s="51"/>
       <c r="B84" s="51"/>
       <c r="C84" s="51"/>
@@ -4688,7 +4688,7 @@
       <c r="Y84" s="51"/>
       <c r="Z84" s="51"/>
     </row>
-    <row r="85" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A85" s="51"/>
       <c r="B85" s="51"/>
       <c r="C85" s="51"/>
@@ -4716,7 +4716,7 @@
       <c r="Y85" s="51"/>
       <c r="Z85" s="51"/>
     </row>
-    <row r="86" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A86" s="51"/>
       <c r="B86" s="51"/>
       <c r="C86" s="51"/>
@@ -4744,7 +4744,7 @@
       <c r="Y86" s="51"/>
       <c r="Z86" s="51"/>
     </row>
-    <row r="87" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A87" s="51"/>
       <c r="B87" s="51"/>
       <c r="C87" s="51"/>
@@ -4772,7 +4772,7 @@
       <c r="Y87" s="51"/>
       <c r="Z87" s="51"/>
     </row>
-    <row r="88" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A88" s="51"/>
       <c r="B88" s="51"/>
       <c r="C88" s="51"/>
@@ -4800,7 +4800,7 @@
       <c r="Y88" s="51"/>
       <c r="Z88" s="51"/>
     </row>
-    <row r="89" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A89" s="51"/>
       <c r="B89" s="51"/>
       <c r="C89" s="51"/>
@@ -4828,7 +4828,7 @@
       <c r="Y89" s="51"/>
       <c r="Z89" s="51"/>
     </row>
-    <row r="90" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A90" s="51"/>
       <c r="B90" s="51"/>
       <c r="C90" s="51"/>
@@ -4856,7 +4856,7 @@
       <c r="Y90" s="51"/>
       <c r="Z90" s="51"/>
     </row>
-    <row r="91" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A91" s="51"/>
       <c r="B91" s="51"/>
       <c r="C91" s="51"/>
@@ -4884,7 +4884,7 @@
       <c r="Y91" s="51"/>
       <c r="Z91" s="51"/>
     </row>
-    <row r="92" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A92" s="51"/>
       <c r="B92" s="51"/>
       <c r="C92" s="51"/>
@@ -4912,7 +4912,7 @@
       <c r="Y92" s="51"/>
       <c r="Z92" s="51"/>
     </row>
-    <row r="93" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A93" s="51"/>
       <c r="B93" s="51"/>
       <c r="C93" s="51"/>
@@ -4940,7 +4940,7 @@
       <c r="Y93" s="51"/>
       <c r="Z93" s="51"/>
     </row>
-    <row r="94" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A94" s="51"/>
       <c r="B94" s="51"/>
       <c r="C94" s="51"/>
@@ -4968,7 +4968,7 @@
       <c r="Y94" s="51"/>
       <c r="Z94" s="51"/>
     </row>
-    <row r="95" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A95" s="51"/>
       <c r="B95" s="51"/>
       <c r="C95" s="51"/>
@@ -4996,7 +4996,7 @@
       <c r="Y95" s="51"/>
       <c r="Z95" s="51"/>
     </row>
-    <row r="96" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A96" s="51"/>
       <c r="B96" s="51"/>
       <c r="C96" s="51"/>
@@ -5024,7 +5024,7 @@
       <c r="Y96" s="51"/>
       <c r="Z96" s="51"/>
     </row>
-    <row r="97" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A97" s="51"/>
       <c r="B97" s="51"/>
       <c r="C97" s="51"/>
@@ -5052,7 +5052,7 @@
       <c r="Y97" s="51"/>
       <c r="Z97" s="51"/>
     </row>
-    <row r="98" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A98" s="51"/>
       <c r="B98" s="51"/>
       <c r="C98" s="51"/>
@@ -5080,7 +5080,7 @@
       <c r="Y98" s="51"/>
       <c r="Z98" s="51"/>
     </row>
-    <row r="99" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A99" s="51"/>
       <c r="B99" s="51"/>
       <c r="C99" s="51"/>
@@ -5139,40 +5139,40 @@
       <selection activeCell="O31" sqref="O31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.109375" style="7" customWidth="1"/>
-    <col min="2" max="2" width="11.6640625" style="7" customWidth="1"/>
-    <col min="3" max="3" width="3.109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.5546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.44140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.88671875" style="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.88671875" style="7" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.44140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="5.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.5546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="6.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.5546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="7.33203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="5.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="6.109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="5.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="5.5546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="5.88671875" style="7" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="6.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="4.88671875" style="7" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="7.5546875" style="7" customWidth="1"/>
-    <col min="25" max="25" width="6.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="6.109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.140625" style="7" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" style="7" customWidth="1"/>
+    <col min="3" max="3" width="3.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="5.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="5.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="6.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="5.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="5.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="5.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="6.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="4.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="7.5703125" style="7" customWidth="1"/>
+    <col min="25" max="25" width="6.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="6.140625" style="7" bestFit="1" customWidth="1"/>
     <col min="27" max="28" width="6" style="7" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="5.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="6.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="31" max="16384" width="9.109375" style="7"/>
+    <col min="29" max="29" width="5.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="6.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="31" max="16384" width="9.140625" style="7"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
       <c r="C3" s="8" t="str" cm="1">
         <f t="array" ref="C3">INDEX(C5:C7,$A$4)</f>
         <v>IE</v>
@@ -5286,12 +5286,12 @@
         <v>IE-MN</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>36</v>
       </c>
@@ -5406,7 +5406,7 @@
         <v>IE-MN</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>39</v>
       </c>
@@ -5523,7 +5523,7 @@
         <v>*IE-MN</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>40</v>
       </c>
@@ -5640,7 +5640,7 @@
         <v>IE-MN</v>
       </c>
     </row>
-    <row r="10" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
         <v>41</v>
       </c>
@@ -5648,7 +5648,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
         <v>43</v>
       </c>
@@ -5656,7 +5656,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
         <v>44</v>
       </c>
@@ -5664,7 +5664,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
         <v>45</v>
       </c>
@@ -5672,7 +5672,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
         <v>46</v>
       </c>
@@ -5680,7 +5680,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
         <v>47</v>
       </c>
@@ -5688,7 +5688,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>48</v>
       </c>
@@ -5696,7 +5696,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>49</v>
       </c>
@@ -5704,7 +5704,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>50</v>
       </c>
@@ -5712,7 +5712,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>51</v>
       </c>
@@ -5720,7 +5720,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
         <v>52</v>
       </c>
@@ -5728,7 +5728,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
         <v>53</v>
       </c>
@@ -5736,7 +5736,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
         <v>54</v>
       </c>
@@ -5744,7 +5744,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="s">
         <v>55</v>
       </c>
@@ -5752,7 +5752,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="12" t="s">
         <v>56</v>
       </c>
@@ -5760,7 +5760,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="12" t="s">
         <v>57</v>
       </c>
@@ -5768,7 +5768,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="12" t="s">
         <v>58</v>
       </c>
@@ -5776,7 +5776,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="12" t="s">
         <v>59</v>
       </c>
@@ -5784,7 +5784,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="12" t="s">
         <v>60</v>
       </c>
@@ -5792,7 +5792,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="12" t="s">
         <v>61</v>
       </c>
@@ -5800,7 +5800,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="12" t="s">
         <v>62</v>
       </c>
@@ -5808,7 +5808,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="12" t="s">
         <v>63</v>
       </c>
@@ -5816,7 +5816,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="12" t="s">
         <v>64</v>
       </c>
@@ -5824,7 +5824,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="12" t="s">
         <v>65</v>
       </c>
@@ -5832,7 +5832,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="12" t="s">
         <v>66</v>
       </c>
@@ -5840,7 +5840,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="12" t="s">
         <v>67</v>
       </c>
@@ -5848,7 +5848,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="12" t="s">
         <v>68</v>
       </c>
@@ -5856,7 +5856,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="13" t="s">
         <v>69</v>
       </c>
@@ -5882,7 +5882,7 @@
                   </from>
                   <to>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>22860</xdr:colOff>
+                    <xdr:colOff>19050</xdr:colOff>
                     <xdr:row>3</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </to>
@@ -5909,31 +5909,31 @@
       <selection pane="bottomRight" activeCell="B87" sqref="B87"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.33203125" customWidth="1"/>
-    <col min="2" max="2" width="8.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.6640625" customWidth="1"/>
+    <col min="1" max="1" width="22.28515625" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" customWidth="1"/>
     <col min="8" max="12" width="17" bestFit="1" customWidth="1"/>
-    <col min="13" max="15" width="18.88671875" bestFit="1" customWidth="1"/>
-    <col min="16" max="32" width="10.6640625" customWidth="1"/>
-    <col min="33" max="33" width="10.6640625" style="7" customWidth="1"/>
-    <col min="34" max="34" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="7.5546875" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="12.33203125" style="14" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="15" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="32" width="10.7109375" customWidth="1"/>
+    <col min="33" max="33" width="10.7109375" style="7" customWidth="1"/>
+    <col min="34" max="34" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="12.28515625" style="14" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="8.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="17"/>
       <c r="B3" s="17"/>
       <c r="C3" s="18"/>
@@ -5954,7 +5954,7 @@
       <c r="R3" s="17"/>
       <c r="S3" s="17"/>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
         <v>77</v>
       </c>
@@ -6013,7 +6013,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="21.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:19" ht="34.5" x14ac:dyDescent="0.25">
       <c r="A5" s="24" t="s">
         <v>91</v>
       </c>
@@ -6070,7 +6070,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="55.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:19" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="28" t="s">
         <v>101</v>
       </c>
@@ -6123,7 +6123,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="32" t="s">
         <v>107</v>
       </c>
@@ -6146,7 +6146,7 @@
       <c r="R7" s="32"/>
       <c r="S7" s="32"/>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="17" t="s">
         <v>120</v>
       </c>
@@ -6205,7 +6205,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="17" t="s">
         <v>123</v>
       </c>
@@ -6264,7 +6264,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="32" t="s">
         <v>108</v>
       </c>
@@ -6287,7 +6287,7 @@
       <c r="R10" s="32"/>
       <c r="S10" s="32"/>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="17" t="s">
         <v>125</v>
       </c>
@@ -6346,7 +6346,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="17" t="s">
         <v>127</v>
       </c>
@@ -6405,7 +6405,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="17" t="s">
         <v>129</v>
       </c>
@@ -6464,7 +6464,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="17" t="s">
         <v>131</v>
       </c>
@@ -6523,7 +6523,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="17" t="s">
         <v>133</v>
       </c>
@@ -6582,7 +6582,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="17" t="s">
         <v>134</v>
       </c>
@@ -6641,7 +6641,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" s="17" t="s">
         <v>136</v>
       </c>
@@ -6700,7 +6700,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" s="17" t="s">
         <v>137</v>
       </c>
@@ -6759,7 +6759,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" s="17" t="s">
         <v>138</v>
       </c>
@@ -6818,7 +6818,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" s="17" t="s">
         <v>140</v>
       </c>
@@ -6877,7 +6877,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" s="17" t="s">
         <v>141</v>
       </c>
@@ -6936,7 +6936,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" s="17" t="s">
         <v>142</v>
       </c>
@@ -6995,7 +6995,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23" s="17" t="s">
         <v>144</v>
       </c>
@@ -7054,7 +7054,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24" s="17" t="s">
         <v>145</v>
       </c>
@@ -7113,7 +7113,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25" s="17" t="s">
         <v>146</v>
       </c>
@@ -7172,7 +7172,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A26" s="17" t="s">
         <v>147</v>
       </c>
@@ -7231,7 +7231,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27" s="17" t="s">
         <v>148</v>
       </c>
@@ -7290,7 +7290,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A28" s="17" t="s">
         <v>149</v>
       </c>
@@ -7349,7 +7349,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A29" s="17" t="s">
         <v>150</v>
       </c>
@@ -7408,7 +7408,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A30" s="32" t="s">
         <v>109</v>
       </c>
@@ -7431,7 +7431,7 @@
       <c r="R30" s="32"/>
       <c r="S30" s="32"/>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A31" s="17" t="s">
         <v>151</v>
       </c>
@@ -7490,7 +7490,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A32" s="17" t="s">
         <v>152</v>
       </c>
@@ -7549,7 +7549,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A33" s="17" t="s">
         <v>153</v>
       </c>
@@ -7608,7 +7608,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A34" s="17" t="s">
         <v>154</v>
       </c>
@@ -7667,7 +7667,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A35" s="17" t="s">
         <v>155</v>
       </c>
@@ -7726,7 +7726,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A36" s="17" t="s">
         <v>156</v>
       </c>
@@ -7785,7 +7785,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A37" s="17" t="s">
         <v>157</v>
       </c>
@@ -7844,7 +7844,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A38" s="17" t="s">
         <v>158</v>
       </c>
@@ -7903,7 +7903,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A39" s="17" t="s">
         <v>159</v>
       </c>
@@ -7962,7 +7962,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A40" s="17" t="s">
         <v>160</v>
       </c>
@@ -8021,7 +8021,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="41" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A41" s="17" t="s">
         <v>161</v>
       </c>
@@ -8080,7 +8080,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A42" s="17" t="s">
         <v>162</v>
       </c>
@@ -8139,7 +8139,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="43" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A43" s="17" t="s">
         <v>163</v>
       </c>
@@ -8198,7 +8198,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="44" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A44" s="17" t="s">
         <v>164</v>
       </c>
@@ -8257,7 +8257,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="45" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A45" s="17" t="s">
         <v>165</v>
       </c>
@@ -8316,7 +8316,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="46" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A46" s="17" t="s">
         <v>166</v>
       </c>
@@ -8375,7 +8375,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="47" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A47" s="17" t="s">
         <v>167</v>
       </c>
@@ -8434,7 +8434,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="48" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A48" s="17" t="s">
         <v>168</v>
       </c>
@@ -8493,7 +8493,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A49" s="17" t="s">
         <v>169</v>
       </c>
@@ -8552,7 +8552,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="50" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A50" s="32" t="s">
         <v>110</v>
       </c>
@@ -8575,7 +8575,7 @@
       <c r="R50" s="32"/>
       <c r="S50" s="32"/>
     </row>
-    <row r="51" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A51" s="17" t="s">
         <v>170</v>
       </c>
@@ -8634,7 +8634,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="52" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A52" s="17" t="s">
         <v>171</v>
       </c>
@@ -8693,7 +8693,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="53" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A53" s="17" t="s">
         <v>172</v>
       </c>
@@ -8752,7 +8752,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="54" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A54" s="17" t="s">
         <v>173</v>
       </c>
@@ -8811,7 +8811,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="55" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A55" s="17" t="s">
         <v>174</v>
       </c>
@@ -8870,7 +8870,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="56" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A56" s="32" t="s">
         <v>111</v>
       </c>
@@ -8893,7 +8893,7 @@
       <c r="R56" s="32"/>
       <c r="S56" s="32"/>
     </row>
-    <row r="57" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A57" s="17" t="s">
         <v>175</v>
       </c>
@@ -8952,7 +8952,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="58" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A58" s="17" t="s">
         <v>176</v>
       </c>
@@ -9011,7 +9011,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="59" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A59" s="17" t="s">
         <v>178</v>
       </c>
@@ -9070,7 +9070,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="60" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A60" s="32" t="s">
         <v>112</v>
       </c>
@@ -9093,7 +9093,7 @@
       <c r="R60" s="32"/>
       <c r="S60" s="32"/>
     </row>
-    <row r="61" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A61" s="17" t="s">
         <v>179</v>
       </c>
@@ -9152,7 +9152,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="62" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A62" s="17" t="s">
         <v>181</v>
       </c>
@@ -9211,7 +9211,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="63" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A63" s="17" t="s">
         <v>182</v>
       </c>
@@ -9270,7 +9270,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="64" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A64" s="17" t="s">
         <v>183</v>
       </c>
@@ -9329,7 +9329,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="65" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A65" s="17" t="s">
         <v>184</v>
       </c>
@@ -9388,7 +9388,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="66" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A66" s="17" t="s">
         <v>186</v>
       </c>
@@ -9447,7 +9447,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="67" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A67" s="17" t="s">
         <v>187</v>
       </c>
@@ -9506,7 +9506,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="68" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A68" s="32" t="s">
         <v>113</v>
       </c>
@@ -9529,7 +9529,7 @@
       <c r="R68" s="32"/>
       <c r="S68" s="32"/>
     </row>
-    <row r="69" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A69" s="17" t="s">
         <v>188</v>
       </c>
@@ -9588,7 +9588,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="70" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A70" s="17" t="s">
         <v>189</v>
       </c>
@@ -9647,7 +9647,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="71" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A71" s="17" t="s">
         <v>190</v>
       </c>
@@ -9706,7 +9706,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="72" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A72" s="17" t="s">
         <v>191</v>
       </c>
@@ -9765,7 +9765,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="73" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A73" s="17" t="s">
         <v>192</v>
       </c>
@@ -9824,7 +9824,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="74" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A74" s="17" t="s">
         <v>193</v>
       </c>
@@ -9883,7 +9883,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="75" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A75" s="17" t="s">
         <v>195</v>
       </c>
@@ -9942,7 +9942,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="76" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A76" s="32" t="s">
         <v>114</v>
       </c>
@@ -9965,7 +9965,7 @@
       <c r="R76" s="32"/>
       <c r="S76" s="32"/>
     </row>
-    <row r="77" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A77" s="17" t="s">
         <v>196</v>
       </c>
@@ -10024,7 +10024,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="78" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A78" s="17" t="s">
         <v>197</v>
       </c>
@@ -10083,7 +10083,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="79" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A79" s="17" t="s">
         <v>198</v>
       </c>
@@ -10142,7 +10142,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="80" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A80" s="17" t="s">
         <v>199</v>
       </c>
@@ -10201,7 +10201,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="81" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A81" s="17" t="s">
         <v>200</v>
       </c>
@@ -10260,7 +10260,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="82" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A82" s="17" t="s">
         <v>201</v>
       </c>
@@ -10319,7 +10319,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="83" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A83" s="17" t="s">
         <v>202</v>
       </c>
@@ -10378,7 +10378,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="84" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A84" s="32" t="s">
         <v>115</v>
       </c>
@@ -10401,7 +10401,7 @@
       <c r="R84" s="32"/>
       <c r="S84" s="32"/>
     </row>
-    <row r="85" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A85" s="17" t="s">
         <v>203</v>
       </c>
@@ -10460,7 +10460,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="86" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A86" s="17" t="s">
         <v>204</v>
       </c>
@@ -10519,7 +10519,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="87" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A87" s="17" t="s">
         <v>205</v>
       </c>
@@ -10578,7 +10578,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="88" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A88" s="32" t="s">
         <v>116</v>
       </c>
@@ -10601,7 +10601,7 @@
       <c r="R88" s="32"/>
       <c r="S88" s="32"/>
     </row>
-    <row r="89" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A89" s="17" t="s">
         <v>206</v>
       </c>
@@ -10638,7 +10638,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A90" s="17" t="s">
         <v>209</v>
       </c>
@@ -10675,7 +10675,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A91" s="17" t="s">
         <v>211</v>
       </c>
@@ -10712,7 +10712,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A92" s="32" t="s">
         <v>117</v>
       </c>
@@ -10735,7 +10735,7 @@
       <c r="R92" s="32"/>
       <c r="S92" s="32"/>
     </row>
-    <row r="93" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A93" s="17" t="s">
         <v>214</v>
       </c>
@@ -10772,7 +10772,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A94" s="35" t="s">
         <v>217</v>
       </c>
@@ -10824,13 +10824,13 @@
       <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="6" width="10.109375" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="10.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B3" s="37" t="s">
         <v>226</v>
       </c>
@@ -10839,7 +10839,7 @@
       <c r="E3" s="38"/>
       <c r="F3" s="38"/>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B4" s="41"/>
       <c r="C4" s="42">
         <v>2020</v>
@@ -10854,7 +10854,7 @@
         <v>2045</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" s="37" t="s">
         <v>219</v>
       </c>
@@ -10871,7 +10871,7 @@
         <v>1.0152168550200416</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" s="37" t="s">
         <v>219</v>
       </c>
@@ -10888,7 +10888,7 @@
         <v>0.99950497151451945</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" s="37" t="s">
         <v>219</v>
       </c>
@@ -10905,7 +10905,7 @@
         <v>0.97549719420789438</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B8" s="37" t="s">
         <v>220</v>
       </c>
@@ -10922,7 +10922,7 @@
         <v>0.99346955426624672</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B9" s="37" t="s">
         <v>220</v>
       </c>
@@ -10939,7 +10939,7 @@
         <v>0.98031421316297396</v>
       </c>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" s="37" t="s">
         <v>220</v>
       </c>
@@ -10956,7 +10956,7 @@
         <v>0.95900971346193919</v>
       </c>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" s="37" t="s">
         <v>221</v>
       </c>
@@ -10973,7 +10973,7 @@
         <v>1.1365210128187446</v>
       </c>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B12" s="37" t="s">
         <v>221</v>
       </c>
@@ -10990,7 +10990,7 @@
         <v>1.1154653616406478</v>
       </c>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B13" s="37" t="s">
         <v>221</v>
       </c>
@@ -11007,7 +11007,7 @@
         <v>1.0762352842237271</v>
       </c>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B14" s="37" t="s">
         <v>222</v>
       </c>
@@ -11024,7 +11024,7 @@
         <v>1.1144919805829321</v>
       </c>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B15" s="37" t="s">
         <v>222</v>
       </c>
@@ -11041,7 +11041,7 @@
         <v>1.0959457863813349</v>
       </c>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B16" s="37" t="s">
         <v>222</v>
       </c>
@@ -11058,7 +11058,7 @@
         <v>1.0594421546674553</v>
       </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" s="37" t="s">
         <v>223</v>
       </c>
@@ -11075,7 +11075,7 @@
         <v>1.2604972977468007</v>
       </c>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B18" s="37" t="s">
         <v>223</v>
       </c>
@@ -11092,7 +11092,7 @@
         <v>1.2339835364748879</v>
       </c>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B19" s="37" t="s">
         <v>223</v>
       </c>
@@ -11109,7 +11109,7 @@
         <v>1.1791965278222314</v>
       </c>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B20" s="37" t="s">
         <v>224</v>
       </c>
@@ -11126,7 +11126,7 @@
         <v>1.2348089941373108</v>
       </c>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B21" s="37" t="s">
         <v>224</v>
       </c>
@@ -11143,7 +11143,7 @@
         <v>1.2108943927694757</v>
       </c>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B22" s="40" t="s">
         <v>224</v>
       </c>
@@ -11160,7 +11160,7 @@
         <v>1.1592783829087885</v>
       </c>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B23" s="43" t="s">
         <v>225</v>
       </c>
@@ -11179,30 +11179,30 @@
       <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.33203125" customWidth="1"/>
-    <col min="6" max="6" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="37.88671875" bestFit="1" customWidth="1"/>
-    <col min="9" max="34" width="10.6640625" customWidth="1"/>
-    <col min="35" max="35" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="36" max="37" width="8.44140625" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="7.5546875" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="41" max="42" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.28515625" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="37.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="34" width="10.7109375" customWidth="1"/>
+    <col min="35" max="35" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="36" max="37" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="41" max="42" width="8.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>8</v>
       </c>
@@ -11214,7 +11214,7 @@
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
     </row>
-    <row r="5" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="4" t="s">
         <v>5</v>
       </c>
@@ -11240,7 +11240,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B6" s="14"/>
       <c r="C6" s="14"/>
       <c r="D6" s="14" t="s">
@@ -11261,7 +11261,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="7" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D7" s="14" t="s">
         <v>70</v>
       </c>
@@ -11279,7 +11279,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D8" s="14" t="s">
         <v>70</v>
       </c>
@@ -11298,7 +11298,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B9" s="45"/>
       <c r="C9" s="45"/>
       <c r="D9" s="45" t="s">
@@ -11319,7 +11319,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B10" s="16"/>
       <c r="C10" s="16"/>
       <c r="D10" s="16" t="s">
@@ -11340,7 +11340,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="14"/>
       <c r="B11" s="14"/>
       <c r="C11" s="14"/>
@@ -11362,7 +11362,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="14"/>
       <c r="B12" s="14"/>
       <c r="C12" s="14"/>
@@ -11384,7 +11384,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="14"/>
       <c r="B13" s="14"/>
       <c r="C13" s="14"/>
@@ -11406,7 +11406,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="14"/>
       <c r="B14" s="14"/>
       <c r="C14" s="14"/>
@@ -11428,7 +11428,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B15" s="16"/>
       <c r="C15" s="16"/>
       <c r="D15" s="16" t="s">
@@ -11449,7 +11449,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B16" s="14"/>
       <c r="C16" s="14"/>
       <c r="D16" s="14" t="s">
@@ -11470,7 +11470,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17" s="14"/>
       <c r="C17" s="14"/>
       <c r="D17" s="14" t="s">
@@ -11491,7 +11491,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B18" s="14"/>
       <c r="C18" s="14"/>
       <c r="D18" s="14" t="s">
@@ -11512,7 +11512,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B19" s="14"/>
       <c r="C19" s="14"/>
       <c r="D19" s="45" t="s">
@@ -11533,7 +11533,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B20" s="16"/>
       <c r="C20" s="16"/>
       <c r="D20" s="16" t="s">
@@ -11554,7 +11554,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D21" s="14" t="s">
         <v>70</v>
       </c>
@@ -11573,7 +11573,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D22" s="14" t="s">
         <v>70</v>
       </c>
@@ -11592,7 +11592,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D23" s="14" t="s">
         <v>70</v>
       </c>
@@ -11611,7 +11611,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D24" s="45" t="s">
         <v>70</v>
       </c>
@@ -11630,7 +11630,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B25" s="16"/>
       <c r="C25" s="16"/>
       <c r="D25" s="16" t="s">
@@ -11651,7 +11651,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
       <c r="H26" s="17"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add James to some cover sheets
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_TRA_EV_Parity.xlsx
+++ b/SuppXLS/Scen_B_TRA_EV_Parity.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CE92432-3F97-43C3-8590-680A1E96AFDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FF2F6AF-0F7C-494F-A5CB-B81DF25BB577}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="17" r:id="rId1"/>
@@ -293,7 +293,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="249">
   <si>
     <t>Year</t>
   </si>
@@ -1057,6 +1057,9 @@
   </si>
   <si>
     <t>Transport sector (TRA)</t>
+  </si>
+  <si>
+    <t>James Glynn (UCC, james.glynn@ucc.ie)</t>
   </si>
 </sst>
 </file>
@@ -2283,7 +2286,7 @@
   <dimension ref="A1:Z99"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2964,7 +2967,9 @@
     </row>
     <row r="24" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="57"/>
-      <c r="B24" s="65"/>
+      <c r="B24" s="65" t="s">
+        <v>248</v>
+      </c>
       <c r="C24" s="65"/>
       <c r="D24" s="65"/>
       <c r="E24" s="51"/>

</xml_diff>